<commit_message>
2017-06-04	Ver 1.0.0.	TC-001 추가	임현
</commit_message>
<xml_diff>
--- a/doc/4_ 테스트케이스 및 테스트결과보고서/테스트케이스_작성_6_blossom.xlsx
+++ b/doc/4_ 테스트케이스 및 테스트결과보고서/테스트케이스_작성_6_blossom.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12168"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12168" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="이력" sheetId="2" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="44">
   <si>
     <t>TestCase ID</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -157,6 +157,59 @@
   </si>
   <si>
     <t>Blossom</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Ver 1.0.0.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>TC-001 추가</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>임현</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>UC004</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>TC-0001</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>To do List 추가</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>로그인</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>과목 명 : 소프트웨어공학</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1. 과목명에서 소프트웨어 공학을 클릭한다.
+2. 추가 버튼을 클릭한다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>과목 명 : 소프트웨어공학</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Fail</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2017.06.04</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>#934</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -450,7 +503,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -493,9 +546,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
@@ -524,6 +574,15 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -842,8 +901,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D28"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" view="pageBreakPreview" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+    <sheetView showGridLines="0" view="pageBreakPreview" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="D9" sqref="A9:D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
@@ -852,48 +911,56 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="40.200000000000003" x14ac:dyDescent="0.4">
-      <c r="B1" s="20" t="s">
+      <c r="B1" s="19" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="7.5" customHeight="1" x14ac:dyDescent="0.4"/>
     <row r="3" spans="1:4" ht="6.75" customHeight="1" x14ac:dyDescent="0.4"/>
     <row r="4" spans="1:4" ht="21" x14ac:dyDescent="0.4">
-      <c r="D4" s="23" t="s">
+      <c r="D4" s="22" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="54" customHeight="1" x14ac:dyDescent="0.4"/>
     <row r="6" spans="1:4" ht="23.25" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A6" s="24" t="s">
+      <c r="A6" s="23" t="s">
         <v>27</v>
       </c>
-      <c r="B6" s="24"/>
-      <c r="C6" s="24"/>
-      <c r="D6" s="24"/>
+      <c r="B6" s="23"/>
+      <c r="C6" s="23"/>
+      <c r="D6" s="23"/>
     </row>
     <row r="7" spans="1:4" ht="4.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="B7" s="21"/>
+      <c r="B7" s="20"/>
     </row>
     <row r="8" spans="1:4" ht="18" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A8" s="17" t="s">
+      <c r="A8" s="16" t="s">
         <v>14</v>
       </c>
-      <c r="B8" s="18" t="s">
+      <c r="B8" s="17" t="s">
         <v>15</v>
       </c>
-      <c r="C8" s="18" t="s">
+      <c r="C8" s="17" t="s">
         <v>16</v>
       </c>
-      <c r="D8" s="19" t="s">
+      <c r="D8" s="18" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A9" s="14"/>
-      <c r="B9" s="15"/>
-      <c r="C9" s="15"/>
-      <c r="D9" s="16"/>
+      <c r="A9" s="24">
+        <v>42890</v>
+      </c>
+      <c r="B9" s="14" t="s">
+        <v>31</v>
+      </c>
+      <c r="C9" s="14" t="s">
+        <v>32</v>
+      </c>
+      <c r="D9" s="15" t="s">
+        <v>33</v>
+      </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A10" s="9"/>
@@ -1023,9 +1090,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K27"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="7" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F15" sqref="F15"/>
+      <selection pane="bottomLeft" activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
@@ -1035,7 +1102,7 @@
     <col min="3" max="3" width="17.69921875" customWidth="1"/>
     <col min="4" max="4" width="35.5" customWidth="1"/>
     <col min="5" max="5" width="30.69921875" customWidth="1"/>
-    <col min="6" max="6" width="17.69921875" customWidth="1"/>
+    <col min="6" max="6" width="22.8984375" customWidth="1"/>
     <col min="7" max="7" width="25.69921875" customWidth="1"/>
     <col min="8" max="8" width="26.59765625" customWidth="1"/>
     <col min="9" max="9" width="8" customWidth="1"/>
@@ -1052,49 +1119,55 @@
       <c r="B3" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="C3" s="1"/>
+      <c r="C3" s="1">
+        <v>1</v>
+      </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.4">
       <c r="B4" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="C4" s="1"/>
+      <c r="C4" s="1">
+        <v>0</v>
+      </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.4">
       <c r="B5" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="C5" s="1"/>
+      <c r="C5" s="1">
+        <v>1</v>
+      </c>
     </row>
     <row r="7" spans="1:11" ht="21.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B7" s="22" t="s">
+      <c r="B7" s="21" t="s">
         <v>21</v>
       </c>
-      <c r="C7" s="22" t="s">
+      <c r="C7" s="21" t="s">
         <v>0</v>
       </c>
-      <c r="D7" s="22" t="s">
+      <c r="D7" s="21" t="s">
         <v>1</v>
       </c>
-      <c r="E7" s="22" t="s">
+      <c r="E7" s="21" t="s">
         <v>22</v>
       </c>
-      <c r="F7" s="22" t="s">
+      <c r="F7" s="21" t="s">
         <v>2</v>
       </c>
-      <c r="G7" s="22" t="s">
+      <c r="G7" s="21" t="s">
         <v>3</v>
       </c>
-      <c r="H7" s="22" t="s">
+      <c r="H7" s="21" t="s">
         <v>4</v>
       </c>
-      <c r="I7" s="22" t="s">
+      <c r="I7" s="21" t="s">
         <v>5</v>
       </c>
-      <c r="J7" s="22" t="s">
+      <c r="J7" s="21" t="s">
         <v>7</v>
       </c>
-      <c r="K7" s="22" t="s">
+      <c r="K7" s="21" t="s">
         <v>6</v>
       </c>
     </row>
@@ -1130,17 +1203,37 @@
         <v>9</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.4">
-      <c r="B9" s="1"/>
-      <c r="C9" s="1"/>
-      <c r="D9" s="1"/>
-      <c r="E9" s="1"/>
-      <c r="F9" s="1"/>
-      <c r="G9" s="1"/>
-      <c r="H9" s="1"/>
-      <c r="I9" s="1"/>
-      <c r="J9" s="8"/>
-      <c r="K9" s="1"/>
+    <row r="9" spans="1:11" ht="52.2" x14ac:dyDescent="0.4">
+      <c r="B9" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="G9" s="25" t="s">
+        <v>39</v>
+      </c>
+      <c r="H9" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="I9" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="J9" s="26" t="s">
+        <v>42</v>
+      </c>
+      <c r="K9" s="1" t="s">
+        <v>43</v>
+      </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.4">
       <c r="B10" s="1"/>

</xml_diff>

<commit_message>
2017.06.07	Ver 1.0.1.	TC002~TC019 추가	박다빈
</commit_message>
<xml_diff>
--- a/doc/4_ 테스트케이스 및 테스트결과보고서/테스트케이스_작성_6_blossom.xlsx
+++ b/doc/4_ 테스트케이스 및 테스트결과보고서/테스트케이스_작성_6_blossom.xlsx
@@ -1,21 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18067"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\임현\Dropbox\대학교\2017년도 1학기\소프트웨어공학, 한혁수 교수님\Blossom\Git\SE2017_6_blossom\doc\4_ 테스트케이스 및 테스트결과보고서\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12168" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="24240" windowHeight="12165" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="이력" sheetId="2" r:id="rId1"/>
     <sheet name="테스트케이스" sheetId="1" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="171027"/>
+  <calcPr calcId="145621"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="193" uniqueCount="124">
   <si>
     <t>TestCase ID</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -180,15 +175,116 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>To do List 추가</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>로그인</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>과목 명 : 소프트웨어공학</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>과목 명 : 소프트웨어공학</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Fail</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2017.06.04</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>#934</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>UC015</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>TC-0002</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>To do List 항목명 입력</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2017.06.06</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Pass</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>UC016</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>UC017</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>UC018</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>TC-0003</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>TC-0004</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>TC-0005</t>
+  </si>
+  <si>
+    <t>TC-0006</t>
+  </si>
+  <si>
+    <t>TC-0008</t>
+  </si>
+  <si>
+    <t>TC-0009</t>
+  </si>
+  <si>
+    <t>To do List 마감기한 입력</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>To do List 중요도 입력</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>To do List 수정</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>UC019</t>
+  </si>
+  <si>
+    <t>UC020</t>
+  </si>
+  <si>
+    <t>UC021</t>
+  </si>
+  <si>
+    <t>To do List 실제마감일 입력</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>To do List 완료여부 입력</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>To do List 삭제</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>과목 추가</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -197,26 +293,255 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>과목 명 : 소프트웨어공학</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Fail</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>2017.06.04</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>#934</t>
+    <t>1. 입력값을 넣는다. 
+2. 추가 버튼을 클릭한다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>설계서</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>O</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>x</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1. 중요에 체크한다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1. 중요에 체크하지 않는다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1. 입력값을 넣는다. 
+2. 수정 버튼을 클릭한다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>to do list 추가</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>소프트웨어공학
+설계서
+2017-05-20
+2017-05-18
+v
+v</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>v</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>TC-0010</t>
+  </si>
+  <si>
+    <t>1. 입력값을 넣는다. 
+2. 삭제 버튼을 클릭한다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>(table에서 일치하는 항목 삭제)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>소프트웨어개발
+설계서
+2017-05-20
+2017-05-18
+v
+v</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>TC-0011</t>
+  </si>
+  <si>
+    <t>table에 아래와 같은 정보로 수정 
+-소프트웨어공학
+-설계서
+-2017-05-20
+-2017-05-18
+-v
+-v</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>변화없음
+(table에서 일치하는 항목이 없어서 삭제되지 않는다.)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>TC-0007</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>TC-0012</t>
+  </si>
+  <si>
+    <t>소프트웨어공학
+설계서
+2017-05-20
+2017-05-18
+v</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>table에 아래와 같은 정보로 수정 
+-소프트웨어공학
+-설계서
+-2017-05-20
+-2017-05-18
+-
+-v</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>UC022</t>
+  </si>
+  <si>
+    <t>To do list 정렬</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1. To do list 버튼을 클릭한다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>To do list에 대해 오름차순으로
+ 정렬</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>TC-0013</t>
+  </si>
+  <si>
+    <t>UC023</t>
+  </si>
+  <si>
+    <t>UC024</t>
+  </si>
+  <si>
+    <t>TC-0014</t>
+  </si>
+  <si>
+    <t>TC-0015</t>
+  </si>
+  <si>
+    <t>To do list 과목명별정렬</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1. 과목명 버튼을 클릭한다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>과목명에 대해 오름차순으로
+ 정렬</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>TC-0016</t>
+  </si>
+  <si>
+    <t>UC025</t>
+  </si>
+  <si>
+    <t>UC026</t>
+  </si>
+  <si>
+    <t>UC027</t>
+  </si>
+  <si>
+    <t>UC028</t>
+  </si>
+  <si>
+    <t>To do list 마감기한별정렬</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>To do list 실제마감일별정렬</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>To do list 완료여부별정렬</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>TC-0017</t>
+  </si>
+  <si>
+    <t>TC-0018</t>
+  </si>
+  <si>
+    <t>TC-0019</t>
+  </si>
+  <si>
+    <t>1. 마감기한 버튼을 클릭한다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>마감기한에 대해 오름차순으로
+ 정렬</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1. 실제마감일 버튼을 클릭한다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>실제마감일에 대해 오름차순으로
+ 정렬</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1. 완료여부 버튼을 클릭한다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>완료여부에 대해 오름차순으로
+ 정렬</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2017.06.07</t>
+  </si>
+  <si>
+    <t>1. 숨김 / 보임 버튼을 클릭한다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>To do list 완료항목 숨기기</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>추가된 모든 to do list 출력</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>완료여부가 O인 항목이 숨겨진 table 출력</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>To do list 완료항목 보이기</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2017.06.06</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -503,7 +828,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -573,9 +898,6 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
@@ -583,14 +905,48 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="표준" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <dxfs count="2">
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFD7D7D7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
+  <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
+    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2">
+      <tableStyleElement type="wholeTable" dxfId="1"/>
+      <tableStyleElement type="headerRow" dxfId="0"/>
+    </tableStyle>
+  </tableStyles>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -891,7 +1247,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -905,12 +1261,12 @@
       <selection activeCell="D9" sqref="A9:D9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="4" width="15.59765625" customWidth="1"/>
+    <col min="1" max="4" width="15.625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="40.200000000000003" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:4" ht="41.25" x14ac:dyDescent="0.3">
       <c r="B1" s="19" t="s">
         <v>26</v>
       </c>
@@ -923,18 +1279,18 @@
       </c>
     </row>
     <row r="5" spans="1:4" ht="54" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="6" spans="1:4" ht="23.25" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A6" s="23" t="s">
+    <row r="6" spans="1:4" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="27" t="s">
         <v>27</v>
       </c>
-      <c r="B6" s="23"/>
-      <c r="C6" s="23"/>
-      <c r="D6" s="23"/>
+      <c r="B6" s="27"/>
+      <c r="C6" s="27"/>
+      <c r="D6" s="27"/>
     </row>
     <row r="7" spans="1:4" ht="4.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B7" s="20"/>
     </row>
-    <row r="8" spans="1:4" ht="18" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:4" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A8" s="16" t="s">
         <v>14</v>
       </c>
@@ -948,8 +1304,8 @@
         <v>17</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A9" s="24">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A9" s="23">
         <v>42890</v>
       </c>
       <c r="B9" s="14" t="s">
@@ -962,115 +1318,115 @@
         <v>33</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:4" ht="17.45" x14ac:dyDescent="0.4">
       <c r="A10" s="9"/>
       <c r="B10" s="1"/>
       <c r="C10" s="1"/>
       <c r="D10" s="10"/>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:4" ht="17.45" x14ac:dyDescent="0.4">
       <c r="A11" s="9"/>
       <c r="B11" s="1"/>
       <c r="C11" s="1"/>
       <c r="D11" s="10"/>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:4" ht="17.45" x14ac:dyDescent="0.4">
       <c r="A12" s="9"/>
       <c r="B12" s="1"/>
       <c r="C12" s="1"/>
       <c r="D12" s="10"/>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:4" ht="17.45" x14ac:dyDescent="0.4">
       <c r="A13" s="9"/>
       <c r="B13" s="1"/>
       <c r="C13" s="1"/>
       <c r="D13" s="10"/>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:4" ht="17.45" x14ac:dyDescent="0.4">
       <c r="A14" s="9"/>
       <c r="B14" s="1"/>
       <c r="C14" s="1"/>
       <c r="D14" s="10"/>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:4" ht="17.45" x14ac:dyDescent="0.4">
       <c r="A15" s="9"/>
       <c r="B15" s="1"/>
       <c r="C15" s="1"/>
       <c r="D15" s="10"/>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="16" spans="1:4" ht="17.45" x14ac:dyDescent="0.4">
       <c r="A16" s="9"/>
       <c r="B16" s="1"/>
       <c r="C16" s="1"/>
       <c r="D16" s="10"/>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="17" spans="1:4" ht="17.45" x14ac:dyDescent="0.4">
       <c r="A17" s="9"/>
       <c r="B17" s="1"/>
       <c r="C17" s="1"/>
       <c r="D17" s="10"/>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="18" spans="1:4" ht="17.45" x14ac:dyDescent="0.4">
       <c r="A18" s="9"/>
       <c r="B18" s="1"/>
       <c r="C18" s="1"/>
       <c r="D18" s="10"/>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="19" spans="1:4" ht="17.45" x14ac:dyDescent="0.4">
       <c r="A19" s="9"/>
       <c r="B19" s="1"/>
       <c r="C19" s="1"/>
       <c r="D19" s="10"/>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="20" spans="1:4" ht="17.45" x14ac:dyDescent="0.4">
       <c r="A20" s="9"/>
       <c r="B20" s="1"/>
       <c r="C20" s="1"/>
       <c r="D20" s="10"/>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="21" spans="1:4" ht="17.45" x14ac:dyDescent="0.4">
       <c r="A21" s="9"/>
       <c r="B21" s="1"/>
       <c r="C21" s="1"/>
       <c r="D21" s="10"/>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="22" spans="1:4" ht="17.45" x14ac:dyDescent="0.4">
       <c r="A22" s="9"/>
       <c r="B22" s="1"/>
       <c r="C22" s="1"/>
       <c r="D22" s="10"/>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="23" spans="1:4" ht="17.45" x14ac:dyDescent="0.4">
       <c r="A23" s="9"/>
       <c r="B23" s="1"/>
       <c r="C23" s="1"/>
       <c r="D23" s="10"/>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="24" spans="1:4" ht="17.45" x14ac:dyDescent="0.4">
       <c r="A24" s="9"/>
       <c r="B24" s="1"/>
       <c r="C24" s="1"/>
       <c r="D24" s="10"/>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="25" spans="1:4" ht="17.45" x14ac:dyDescent="0.4">
       <c r="A25" s="9"/>
       <c r="B25" s="1"/>
       <c r="C25" s="1"/>
       <c r="D25" s="10"/>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A26" s="9"/>
       <c r="B26" s="1"/>
       <c r="C26" s="1"/>
       <c r="D26" s="10"/>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A27" s="9"/>
       <c r="B27" s="1"/>
       <c r="C27" s="1"/>
       <c r="D27" s="10"/>
     </row>
-    <row r="28" spans="1:4" ht="18" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="28" spans="1:4" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A28" s="11"/>
       <c r="B28" s="12"/>
       <c r="C28" s="12"/>
@@ -1088,26 +1444,26 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K27"/>
+  <dimension ref="A1:K37"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="7" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D3" sqref="D3"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane ySplit="7" topLeftCell="A23" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="J25" sqref="J25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="5.19921875" customWidth="1"/>
-    <col min="2" max="2" width="16.59765625" customWidth="1"/>
-    <col min="3" max="3" width="17.69921875" customWidth="1"/>
+    <col min="1" max="1" width="5.25" customWidth="1"/>
+    <col min="2" max="2" width="16.625" customWidth="1"/>
+    <col min="3" max="3" width="17.75" customWidth="1"/>
     <col min="4" max="4" width="35.5" customWidth="1"/>
-    <col min="5" max="5" width="30.69921875" customWidth="1"/>
-    <col min="6" max="6" width="22.8984375" customWidth="1"/>
-    <col min="7" max="7" width="25.69921875" customWidth="1"/>
-    <col min="8" max="8" width="26.59765625" customWidth="1"/>
+    <col min="5" max="5" width="30.75" customWidth="1"/>
+    <col min="6" max="6" width="22.875" customWidth="1"/>
+    <col min="7" max="7" width="25.75" customWidth="1"/>
+    <col min="8" max="8" width="26.625" customWidth="1"/>
     <col min="9" max="9" width="8" customWidth="1"/>
-    <col min="10" max="10" width="11.8984375" style="7" customWidth="1"/>
-    <col min="11" max="11" width="17.69921875" customWidth="1"/>
+    <col min="10" max="10" width="11.875" style="7" customWidth="1"/>
+    <col min="11" max="11" width="17.75" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="30" x14ac:dyDescent="0.4">
@@ -1115,23 +1471,23 @@
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B3" s="2" t="s">
         <v>10</v>
       </c>
       <c r="C3" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.4">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B4" s="2" t="s">
         <v>11</v>
       </c>
       <c r="C4" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.4">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B5" s="2" t="s">
         <v>12</v>
       </c>
@@ -1139,7 +1495,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:11" ht="21.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:11" ht="21.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B7" s="21" t="s">
         <v>21</v>
       </c>
@@ -1171,7 +1527,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:11" ht="87" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:11" ht="82.5" x14ac:dyDescent="0.3">
       <c r="B8" s="4" t="s">
         <v>28</v>
       </c>
@@ -1203,7 +1559,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="9" spans="1:11" ht="52.2" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:11" ht="49.5" x14ac:dyDescent="0.3">
       <c r="B9" s="1" t="s">
         <v>34</v>
       </c>
@@ -1211,245 +1567,671 @@
         <v>35</v>
       </c>
       <c r="D9" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="E9" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="E9" s="1" t="s">
+      <c r="F9" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="F9" s="1" t="s">
+      <c r="G9" s="24" t="s">
+        <v>66</v>
+      </c>
+      <c r="H9" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="G9" s="25" t="s">
+      <c r="I9" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="H9" s="1" t="s">
+      <c r="J9" s="25" t="s">
         <v>40</v>
       </c>
-      <c r="I9" s="1" t="s">
+      <c r="K9" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="J9" s="26" t="s">
+    </row>
+    <row r="10" spans="1:11" ht="33" x14ac:dyDescent="0.3">
+      <c r="B10" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="K9" s="1" t="s">
+      <c r="C10" s="1" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.4">
-      <c r="B10" s="1"/>
-      <c r="C10" s="1"/>
-      <c r="D10" s="1"/>
-      <c r="E10" s="1"/>
-      <c r="F10" s="1"/>
-      <c r="G10" s="1"/>
-      <c r="H10" s="1"/>
-      <c r="I10" s="1"/>
-      <c r="J10" s="8"/>
+      <c r="D10" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="G10" s="24" t="s">
+        <v>67</v>
+      </c>
+      <c r="H10" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="I10" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="J10" s="25" t="s">
+        <v>45</v>
+      </c>
       <c r="K10" s="1"/>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.4">
-      <c r="B11" s="1"/>
-      <c r="C11" s="1"/>
-      <c r="D11" s="1"/>
-      <c r="E11" s="1"/>
-      <c r="F11" s="1"/>
-      <c r="G11" s="1"/>
-      <c r="H11" s="1"/>
-      <c r="I11" s="1"/>
-      <c r="J11" s="8"/>
+    <row r="11" spans="1:11" ht="33" x14ac:dyDescent="0.3">
+      <c r="B11" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="F11" s="26">
+        <v>42875</v>
+      </c>
+      <c r="G11" s="24" t="s">
+        <v>67</v>
+      </c>
+      <c r="H11" s="26">
+        <v>42875</v>
+      </c>
+      <c r="I11" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="J11" s="25" t="s">
+        <v>45</v>
+      </c>
       <c r="K11" s="1"/>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.4">
-      <c r="B12" s="1"/>
-      <c r="C12" s="1"/>
-      <c r="D12" s="1"/>
-      <c r="E12" s="1"/>
-      <c r="F12" s="1"/>
-      <c r="G12" s="1"/>
-      <c r="H12" s="1"/>
-      <c r="I12" s="1"/>
-      <c r="J12" s="8"/>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="B12" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="F12" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="G12" s="24" t="s">
+        <v>71</v>
+      </c>
+      <c r="H12" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="I12" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="J12" s="25" t="s">
+        <v>45</v>
+      </c>
       <c r="K12" s="1"/>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.4">
-      <c r="B13" s="1"/>
-      <c r="C13" s="1"/>
-      <c r="D13" s="1"/>
-      <c r="E13" s="1"/>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="B13" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>36</v>
+      </c>
       <c r="F13" s="1"/>
-      <c r="G13" s="1"/>
-      <c r="H13" s="1"/>
-      <c r="I13" s="1"/>
-      <c r="J13" s="8"/>
+      <c r="G13" s="24" t="s">
+        <v>72</v>
+      </c>
+      <c r="H13" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="I13" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="J13" s="25" t="s">
+        <v>45</v>
+      </c>
       <c r="K13" s="1"/>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.4">
-      <c r="B14" s="1"/>
-      <c r="C14" s="1"/>
-      <c r="D14" s="1"/>
-      <c r="E14" s="1"/>
-      <c r="F14" s="1"/>
-      <c r="G14" s="1"/>
-      <c r="H14" s="1"/>
-      <c r="I14" s="1"/>
-      <c r="J14" s="8"/>
+    <row r="14" spans="1:11" ht="132" x14ac:dyDescent="0.3">
+      <c r="B14" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="F14" s="24" t="s">
+        <v>75</v>
+      </c>
+      <c r="G14" s="24" t="s">
+        <v>73</v>
+      </c>
+      <c r="H14" s="24" t="s">
+        <v>82</v>
+      </c>
+      <c r="I14" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="J14" s="25" t="s">
+        <v>45</v>
+      </c>
       <c r="K14" s="1"/>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.4">
-      <c r="B15" s="1"/>
-      <c r="C15" s="1"/>
-      <c r="D15" s="1"/>
-      <c r="E15" s="1"/>
-      <c r="F15" s="1"/>
-      <c r="G15" s="1"/>
-      <c r="H15" s="1"/>
-      <c r="I15" s="1"/>
-      <c r="J15" s="8"/>
+    <row r="15" spans="1:11" ht="132" x14ac:dyDescent="0.3">
+      <c r="B15" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="F15" s="24" t="s">
+        <v>86</v>
+      </c>
+      <c r="G15" s="24" t="s">
+        <v>73</v>
+      </c>
+      <c r="H15" s="24" t="s">
+        <v>87</v>
+      </c>
+      <c r="I15" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="J15" s="25" t="s">
+        <v>45</v>
+      </c>
       <c r="K15" s="1"/>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.4">
-      <c r="B16" s="1"/>
-      <c r="C16" s="1"/>
-      <c r="D16" s="1"/>
-      <c r="E16" s="1"/>
-      <c r="F16" s="1"/>
-      <c r="G16" s="1"/>
-      <c r="H16" s="1"/>
-      <c r="I16" s="1"/>
-      <c r="J16" s="8"/>
+    <row r="16" spans="1:11" ht="33" x14ac:dyDescent="0.3">
+      <c r="B16" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="F16" s="26">
+        <v>42874</v>
+      </c>
+      <c r="G16" s="24" t="s">
+        <v>67</v>
+      </c>
+      <c r="H16" s="26">
+        <v>42874</v>
+      </c>
+      <c r="I16" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="J16" s="25" t="s">
+        <v>45</v>
+      </c>
       <c r="K16" s="1"/>
     </row>
-    <row r="17" spans="2:11" x14ac:dyDescent="0.4">
-      <c r="B17" s="1"/>
-      <c r="C17" s="1"/>
-      <c r="D17" s="1"/>
-      <c r="E17" s="1"/>
-      <c r="F17" s="1"/>
-      <c r="G17" s="1"/>
-      <c r="H17" s="1"/>
-      <c r="I17" s="1"/>
-      <c r="J17" s="8"/>
+    <row r="17" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B17" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="F17" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="G17" s="24" t="s">
+        <v>71</v>
+      </c>
+      <c r="H17" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="I17" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="J17" s="25" t="s">
+        <v>45</v>
+      </c>
       <c r="K17" s="1"/>
     </row>
-    <row r="18" spans="2:11" x14ac:dyDescent="0.4">
-      <c r="B18" s="1"/>
-      <c r="C18" s="1"/>
-      <c r="D18" s="1"/>
-      <c r="E18" s="1"/>
+    <row r="18" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B18" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>36</v>
+      </c>
       <c r="F18" s="1"/>
-      <c r="G18" s="1"/>
-      <c r="H18" s="1"/>
-      <c r="I18" s="1"/>
-      <c r="J18" s="8"/>
+      <c r="G18" s="24" t="s">
+        <v>72</v>
+      </c>
+      <c r="H18" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="I18" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="J18" s="25" t="s">
+        <v>45</v>
+      </c>
       <c r="K18" s="1"/>
     </row>
-    <row r="19" spans="2:11" x14ac:dyDescent="0.4">
-      <c r="B19" s="1"/>
-      <c r="C19" s="1"/>
-      <c r="D19" s="1"/>
-      <c r="E19" s="1"/>
-      <c r="F19" s="1"/>
-      <c r="G19" s="1"/>
-      <c r="H19" s="1"/>
-      <c r="I19" s="1"/>
-      <c r="J19" s="8"/>
+    <row r="19" spans="2:11" ht="99" x14ac:dyDescent="0.3">
+      <c r="B19" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="F19" s="24" t="s">
+        <v>75</v>
+      </c>
+      <c r="G19" s="24" t="s">
+        <v>78</v>
+      </c>
+      <c r="H19" s="24" t="s">
+        <v>79</v>
+      </c>
+      <c r="I19" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="J19" s="25" t="s">
+        <v>45</v>
+      </c>
       <c r="K19" s="1"/>
     </row>
-    <row r="20" spans="2:11" x14ac:dyDescent="0.4">
-      <c r="B20" s="1"/>
-      <c r="C20" s="1"/>
-      <c r="D20" s="1"/>
-      <c r="E20" s="1"/>
-      <c r="F20" s="1"/>
-      <c r="G20" s="1"/>
-      <c r="H20" s="1"/>
-      <c r="I20" s="1"/>
-      <c r="J20" s="8"/>
+    <row r="20" spans="2:11" ht="99" x14ac:dyDescent="0.3">
+      <c r="B20" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="E20" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="F20" s="24" t="s">
+        <v>80</v>
+      </c>
+      <c r="G20" s="24" t="s">
+        <v>78</v>
+      </c>
+      <c r="H20" s="24" t="s">
+        <v>83</v>
+      </c>
+      <c r="I20" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="J20" s="25" t="s">
+        <v>45</v>
+      </c>
       <c r="K20" s="1"/>
     </row>
-    <row r="21" spans="2:11" x14ac:dyDescent="0.4">
-      <c r="B21" s="1"/>
-      <c r="C21" s="1"/>
-      <c r="D21" s="1"/>
-      <c r="E21" s="1"/>
+    <row r="21" spans="2:11" ht="49.5" x14ac:dyDescent="0.3">
+      <c r="B21" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="E21" s="1" t="s">
+        <v>74</v>
+      </c>
       <c r="F21" s="1"/>
-      <c r="G21" s="1"/>
-      <c r="H21" s="1"/>
-      <c r="I21" s="1"/>
-      <c r="J21" s="8"/>
+      <c r="G21" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="H21" s="24" t="s">
+        <v>91</v>
+      </c>
+      <c r="I21" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="J21" s="25" t="s">
+        <v>45</v>
+      </c>
       <c r="K21" s="1"/>
     </row>
-    <row r="22" spans="2:11" x14ac:dyDescent="0.4">
-      <c r="B22" s="1"/>
-      <c r="C22" s="1"/>
-      <c r="D22" s="1"/>
-      <c r="E22" s="1"/>
+    <row r="22" spans="2:11" ht="33" x14ac:dyDescent="0.3">
+      <c r="B22" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="E22" s="1" t="s">
+        <v>74</v>
+      </c>
       <c r="F22" s="1"/>
-      <c r="G22" s="1"/>
-      <c r="H22" s="1"/>
-      <c r="I22" s="1"/>
-      <c r="J22" s="8"/>
+      <c r="G22" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="H22" s="24" t="s">
+        <v>99</v>
+      </c>
+      <c r="I22" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="J22" s="25" t="s">
+        <v>45</v>
+      </c>
       <c r="K22" s="1"/>
     </row>
-    <row r="23" spans="2:11" x14ac:dyDescent="0.4">
-      <c r="B23" s="1"/>
-      <c r="C23" s="1"/>
-      <c r="D23" s="1"/>
-      <c r="E23" s="1"/>
+    <row r="23" spans="2:11" ht="33" x14ac:dyDescent="0.3">
+      <c r="B23" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="E23" s="1" t="s">
+        <v>74</v>
+      </c>
       <c r="F23" s="1"/>
-      <c r="G23" s="1"/>
-      <c r="H23" s="1"/>
-      <c r="I23" s="1"/>
-      <c r="J23" s="8"/>
+      <c r="G23" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="H23" s="24" t="s">
+        <v>112</v>
+      </c>
+      <c r="I23" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="J23" s="25" t="s">
+        <v>45</v>
+      </c>
       <c r="K23" s="1"/>
     </row>
-    <row r="24" spans="2:11" x14ac:dyDescent="0.4">
-      <c r="B24" s="1"/>
-      <c r="C24" s="1"/>
-      <c r="D24" s="1"/>
-      <c r="E24" s="1"/>
+    <row r="24" spans="2:11" ht="49.5" x14ac:dyDescent="0.3">
+      <c r="B24" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="D24" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="E24" s="1" t="s">
+        <v>74</v>
+      </c>
       <c r="F24" s="1"/>
-      <c r="G24" s="1"/>
-      <c r="H24" s="1"/>
-      <c r="I24" s="1"/>
-      <c r="J24" s="8"/>
+      <c r="G24" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="H24" s="24" t="s">
+        <v>114</v>
+      </c>
+      <c r="I24" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="J24" s="25" t="s">
+        <v>45</v>
+      </c>
       <c r="K24" s="1"/>
     </row>
-    <row r="25" spans="2:11" x14ac:dyDescent="0.4">
-      <c r="B25" s="1"/>
-      <c r="C25" s="1"/>
-      <c r="D25" s="1"/>
-      <c r="E25" s="1"/>
+    <row r="25" spans="2:11" ht="33" x14ac:dyDescent="0.3">
+      <c r="B25" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="D25" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="E25" s="1" t="s">
+        <v>74</v>
+      </c>
       <c r="F25" s="1"/>
-      <c r="G25" s="1"/>
-      <c r="H25" s="1"/>
-      <c r="I25" s="1"/>
-      <c r="J25" s="8"/>
+      <c r="G25" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="H25" s="24" t="s">
+        <v>116</v>
+      </c>
+      <c r="I25" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="J25" s="25" t="s">
+        <v>123</v>
+      </c>
       <c r="K25" s="1"/>
     </row>
-    <row r="26" spans="2:11" x14ac:dyDescent="0.4">
-      <c r="B26" s="1"/>
-      <c r="C26" s="1"/>
-      <c r="D26" s="1"/>
-      <c r="E26" s="1"/>
+    <row r="26" spans="2:11" ht="33" x14ac:dyDescent="0.3">
+      <c r="B26" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="D26" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="E26" s="1" t="s">
+        <v>74</v>
+      </c>
       <c r="F26" s="1"/>
-      <c r="G26" s="1"/>
-      <c r="H26" s="1"/>
-      <c r="I26" s="1"/>
-      <c r="J26" s="8"/>
+      <c r="G26" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="H26" s="24" t="s">
+        <v>121</v>
+      </c>
+      <c r="I26" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="J26" s="25" t="s">
+        <v>117</v>
+      </c>
       <c r="K26" s="1"/>
     </row>
-    <row r="27" spans="2:11" x14ac:dyDescent="0.4">
-      <c r="B27" s="1"/>
-      <c r="C27" s="1"/>
-      <c r="D27" s="1"/>
-      <c r="E27" s="1"/>
+    <row r="27" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B27" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="D27" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="E27" s="1" t="s">
+        <v>74</v>
+      </c>
       <c r="F27" s="1"/>
-      <c r="G27" s="1"/>
-      <c r="H27" s="1"/>
-      <c r="I27" s="1"/>
-      <c r="J27" s="8"/>
+      <c r="G27" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="H27" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="I27" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="J27" s="25" t="s">
+        <v>117</v>
+      </c>
       <c r="K27" s="1"/>
+    </row>
+    <row r="28" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B28" s="1"/>
+      <c r="C28" s="1"/>
+      <c r="D28" s="1"/>
+      <c r="E28" s="1"/>
+      <c r="F28" s="1"/>
+      <c r="G28" s="1"/>
+      <c r="H28" s="1"/>
+      <c r="I28" s="1"/>
+      <c r="J28" s="8"/>
+      <c r="K28" s="1"/>
+    </row>
+    <row r="29" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B29" s="1"/>
+      <c r="C29" s="1"/>
+      <c r="D29" s="1"/>
+      <c r="E29" s="1"/>
+      <c r="F29" s="1"/>
+      <c r="G29" s="1"/>
+      <c r="H29" s="1"/>
+      <c r="I29" s="1"/>
+      <c r="J29" s="8"/>
+      <c r="K29" s="1"/>
+    </row>
+    <row r="30" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B30" s="1"/>
+      <c r="C30" s="1"/>
+      <c r="D30" s="1"/>
+      <c r="E30" s="1"/>
+      <c r="F30" s="1"/>
+      <c r="G30" s="1"/>
+      <c r="H30" s="1"/>
+      <c r="I30" s="1"/>
+      <c r="J30" s="8"/>
+      <c r="K30" s="1"/>
+    </row>
+    <row r="31" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B31" s="1"/>
+      <c r="C31" s="1"/>
+      <c r="D31" s="1"/>
+      <c r="E31" s="1"/>
+      <c r="F31" s="1"/>
+      <c r="G31" s="1"/>
+      <c r="H31" s="1"/>
+      <c r="I31" s="1"/>
+      <c r="J31" s="8"/>
+      <c r="K31" s="1"/>
+    </row>
+    <row r="32" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B32" s="1"/>
+      <c r="C32" s="1"/>
+      <c r="D32" s="1"/>
+      <c r="E32" s="1"/>
+      <c r="F32" s="1"/>
+      <c r="G32" s="1"/>
+      <c r="H32" s="1"/>
+      <c r="I32" s="1"/>
+      <c r="J32" s="8"/>
+      <c r="K32" s="1"/>
+    </row>
+    <row r="33" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B33" s="1"/>
+      <c r="C33" s="1"/>
+      <c r="D33" s="1"/>
+      <c r="E33" s="1"/>
+      <c r="F33" s="1"/>
+      <c r="G33" s="1"/>
+      <c r="H33" s="1"/>
+      <c r="I33" s="1"/>
+      <c r="J33" s="8"/>
+      <c r="K33" s="1"/>
+    </row>
+    <row r="34" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B34" s="1"/>
+      <c r="C34" s="1"/>
+      <c r="D34" s="1"/>
+      <c r="E34" s="1"/>
+      <c r="F34" s="1"/>
+      <c r="G34" s="1"/>
+      <c r="H34" s="1"/>
+      <c r="I34" s="1"/>
+      <c r="J34" s="8"/>
+      <c r="K34" s="1"/>
+    </row>
+    <row r="35" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B35" s="1"/>
+      <c r="C35" s="1"/>
+      <c r="D35" s="1"/>
+      <c r="E35" s="1"/>
+      <c r="F35" s="1"/>
+      <c r="G35" s="1"/>
+      <c r="H35" s="1"/>
+      <c r="I35" s="1"/>
+      <c r="J35" s="8"/>
+      <c r="K35" s="1"/>
+    </row>
+    <row r="36" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B36" s="1"/>
+      <c r="C36" s="1"/>
+      <c r="D36" s="1"/>
+      <c r="E36" s="1"/>
+      <c r="F36" s="1"/>
+      <c r="G36" s="1"/>
+      <c r="H36" s="1"/>
+      <c r="I36" s="1"/>
+      <c r="J36" s="8"/>
+      <c r="K36" s="1"/>
+    </row>
+    <row r="37" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B37" s="1"/>
+      <c r="C37" s="1"/>
+      <c r="D37" s="1"/>
+      <c r="E37" s="1"/>
+      <c r="F37" s="1"/>
+      <c r="G37" s="1"/>
+      <c r="H37" s="1"/>
+      <c r="I37" s="1"/>
+      <c r="J37" s="8"/>
+      <c r="K37" s="1"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>

</xml_diff>

<commit_message>
2017-06-07	Ver 1.1.0.	테스트 케이스 제출	임현
</commit_message>
<xml_diff>
--- a/doc/4_ 테스트케이스 및 테스트결과보고서/테스트케이스_작성_6_blossom.xlsx
+++ b/doc/4_ 테스트케이스 및 테스트결과보고서/테스트케이스_작성_6_blossom.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17329"/>
-  <workbookPr defaultThemeVersion="164011"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18067"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\사라\Desktop\SE2017_6_blossom\doc\4_ 테스트케이스 및 테스트결과보고서\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\임현\Dropbox\대학교\2017년도 1학기\소프트웨어공학, 한혁수 교수님\Blossom\Git\SE2017_6_blossom\doc\4_ 테스트케이스 및 테스트결과보고서\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24240" windowHeight="12170" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="24240" windowHeight="12168" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="이력" sheetId="2" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="320" uniqueCount="177">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="323" uniqueCount="180">
   <si>
     <t>TestCase ID</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -796,6 +796,18 @@
 2017-05-18
 v
 v</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Ver 1.1.0.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>임현</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>테스트케이스 제출</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1101,7 +1113,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1194,6 +1206,9 @@
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1541,28 +1556,28 @@
   <dimension ref="A1:D28"/>
   <sheetViews>
     <sheetView showGridLines="0" view="pageBreakPreview" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="17" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="4" width="15.58203125" customWidth="1"/>
+    <col min="1" max="4" width="15.59765625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="39.5" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:4" ht="40.200000000000003" x14ac:dyDescent="0.4">
       <c r="B1" s="19" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="7.5" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="3" spans="1:4" ht="6.75" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="4" spans="1:4" ht="21" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:4" ht="7.5" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="3" spans="1:4" ht="6.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="4" spans="1:4" ht="21" x14ac:dyDescent="0.4">
       <c r="D4" s="22" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="54" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="6" spans="1:4" ht="23.25" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:4" ht="54" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="6" spans="1:4" ht="23.25" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A6" s="30" t="s">
         <v>27</v>
       </c>
@@ -1570,10 +1585,10 @@
       <c r="C6" s="30"/>
       <c r="D6" s="30"/>
     </row>
-    <row r="7" spans="1:4" ht="4.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="7" spans="1:4" ht="4.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B7" s="20"/>
     </row>
-    <row r="8" spans="1:4" ht="17.5" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="8" spans="1:4" ht="18" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A8" s="16" t="s">
         <v>14</v>
       </c>
@@ -1587,7 +1602,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A9" s="23">
         <v>42890</v>
       </c>
@@ -1601,115 +1616,123 @@
         <v>33</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A10" s="9"/>
-      <c r="B10" s="1"/>
-      <c r="C10" s="1"/>
-      <c r="D10" s="10"/>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A10" s="31">
+        <v>42893</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>179</v>
+      </c>
+      <c r="D10" s="10" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A11" s="9"/>
       <c r="B11" s="1"/>
       <c r="C11" s="1"/>
       <c r="D11" s="10"/>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A12" s="9"/>
       <c r="B12" s="1"/>
       <c r="C12" s="1"/>
       <c r="D12" s="10"/>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A13" s="9"/>
       <c r="B13" s="1"/>
       <c r="C13" s="1"/>
       <c r="D13" s="10"/>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A14" s="9"/>
       <c r="B14" s="1"/>
       <c r="C14" s="1"/>
       <c r="D14" s="10"/>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A15" s="9"/>
       <c r="B15" s="1"/>
       <c r="C15" s="1"/>
       <c r="D15" s="10"/>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A16" s="9"/>
       <c r="B16" s="1"/>
       <c r="C16" s="1"/>
       <c r="D16" s="10"/>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A17" s="9"/>
       <c r="B17" s="1"/>
       <c r="C17" s="1"/>
       <c r="D17" s="10"/>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A18" s="9"/>
       <c r="B18" s="1"/>
       <c r="C18" s="1"/>
       <c r="D18" s="10"/>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A19" s="9"/>
       <c r="B19" s="1"/>
       <c r="C19" s="1"/>
       <c r="D19" s="10"/>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A20" s="9"/>
       <c r="B20" s="1"/>
       <c r="C20" s="1"/>
       <c r="D20" s="10"/>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A21" s="9"/>
       <c r="B21" s="1"/>
       <c r="C21" s="1"/>
       <c r="D21" s="10"/>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A22" s="9"/>
       <c r="B22" s="1"/>
       <c r="C22" s="1"/>
       <c r="D22" s="10"/>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A23" s="9"/>
       <c r="B23" s="1"/>
       <c r="C23" s="1"/>
       <c r="D23" s="10"/>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A24" s="9"/>
       <c r="B24" s="1"/>
       <c r="C24" s="1"/>
       <c r="D24" s="10"/>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A25" s="9"/>
       <c r="B25" s="1"/>
       <c r="C25" s="1"/>
       <c r="D25" s="10"/>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A26" s="9"/>
       <c r="B26" s="1"/>
       <c r="C26" s="1"/>
       <c r="D26" s="10"/>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A27" s="9"/>
       <c r="B27" s="1"/>
       <c r="C27" s="1"/>
       <c r="D27" s="10"/>
     </row>
-    <row r="28" spans="1:4" ht="17.5" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="28" spans="1:4" ht="18" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A28" s="11"/>
       <c r="B28" s="12"/>
       <c r="C28" s="12"/>
@@ -1730,31 +1753,31 @@
   <dimension ref="A1:K42"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane ySplit="7" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="7" topLeftCell="A38" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="17" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="5.1640625" customWidth="1"/>
-    <col min="2" max="2" width="16.58203125" customWidth="1"/>
-    <col min="3" max="3" width="17.6640625" customWidth="1"/>
+    <col min="1" max="1" width="5.19921875" customWidth="1"/>
+    <col min="2" max="2" width="16.59765625" customWidth="1"/>
+    <col min="3" max="3" width="17.69921875" customWidth="1"/>
     <col min="4" max="4" width="35.5" customWidth="1"/>
-    <col min="5" max="5" width="30.6640625" customWidth="1"/>
-    <col min="6" max="6" width="22.83203125" customWidth="1"/>
-    <col min="7" max="7" width="25.6640625" customWidth="1"/>
-    <col min="8" max="8" width="26.58203125" customWidth="1"/>
+    <col min="5" max="5" width="30.69921875" customWidth="1"/>
+    <col min="6" max="6" width="22.796875" customWidth="1"/>
+    <col min="7" max="7" width="25.69921875" customWidth="1"/>
+    <col min="8" max="8" width="26.59765625" customWidth="1"/>
     <col min="9" max="9" width="8" customWidth="1"/>
-    <col min="10" max="10" width="11.83203125" style="7" customWidth="1"/>
-    <col min="11" max="11" width="17.6640625" customWidth="1"/>
+    <col min="10" max="10" width="11.796875" style="7" customWidth="1"/>
+    <col min="11" max="11" width="17.69921875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="30" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:11" ht="30" x14ac:dyDescent="0.4">
       <c r="A1" s="3" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.4">
       <c r="B3" s="2" t="s">
         <v>10</v>
       </c>
@@ -1762,7 +1785,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.4">
       <c r="B4" s="2" t="s">
         <v>11</v>
       </c>
@@ -1770,7 +1793,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.4">
       <c r="B5" s="2" t="s">
         <v>12</v>
       </c>
@@ -1778,7 +1801,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:11" ht="21.75" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:11" ht="21.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B7" s="21" t="s">
         <v>21</v>
       </c>
@@ -1810,7 +1833,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:11" ht="85" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:11" ht="87" x14ac:dyDescent="0.4">
       <c r="B8" s="4" t="s">
         <v>28</v>
       </c>
@@ -1842,7 +1865,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="9" spans="1:11" ht="51" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:11" ht="52.2" x14ac:dyDescent="0.4">
       <c r="B9" s="1" t="s">
         <v>34</v>
       </c>
@@ -1874,7 +1897,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="10" spans="1:11" ht="51" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:11" ht="52.2" x14ac:dyDescent="0.4">
       <c r="B10" s="1" t="s">
         <v>34</v>
       </c>
@@ -1906,7 +1929,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="11" spans="1:11" ht="34" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:11" ht="34.799999999999997" x14ac:dyDescent="0.4">
       <c r="B11" s="1" t="s">
         <v>42</v>
       </c>
@@ -1936,7 +1959,7 @@
       </c>
       <c r="K11" s="1"/>
     </row>
-    <row r="12" spans="1:11" ht="34" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:11" ht="34.799999999999997" x14ac:dyDescent="0.4">
       <c r="B12" s="1" t="s">
         <v>47</v>
       </c>
@@ -1966,7 +1989,7 @@
       </c>
       <c r="K12" s="1"/>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.4">
       <c r="B13" s="1" t="s">
         <v>48</v>
       </c>
@@ -1996,7 +2019,7 @@
       </c>
       <c r="K13" s="1"/>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.4">
       <c r="B14" s="1" t="s">
         <v>48</v>
       </c>
@@ -2024,7 +2047,7 @@
       </c>
       <c r="K14" s="1"/>
     </row>
-    <row r="15" spans="1:11" ht="136" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:11" ht="139.19999999999999" x14ac:dyDescent="0.4">
       <c r="B15" s="1" t="s">
         <v>49</v>
       </c>
@@ -2054,7 +2077,7 @@
       </c>
       <c r="K15" s="1"/>
     </row>
-    <row r="16" spans="1:11" ht="136" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:11" ht="139.19999999999999" x14ac:dyDescent="0.4">
       <c r="B16" s="1" t="s">
         <v>49</v>
       </c>
@@ -2084,7 +2107,7 @@
       </c>
       <c r="K16" s="1"/>
     </row>
-    <row r="17" spans="2:11" ht="34" x14ac:dyDescent="0.45">
+    <row r="17" spans="2:11" ht="34.799999999999997" x14ac:dyDescent="0.4">
       <c r="B17" s="1" t="s">
         <v>59</v>
       </c>
@@ -2114,7 +2137,7 @@
       </c>
       <c r="K17" s="1"/>
     </row>
-    <row r="18" spans="2:11" x14ac:dyDescent="0.45">
+    <row r="18" spans="2:11" x14ac:dyDescent="0.4">
       <c r="B18" s="1" t="s">
         <v>60</v>
       </c>
@@ -2144,7 +2167,7 @@
       </c>
       <c r="K18" s="1"/>
     </row>
-    <row r="19" spans="2:11" x14ac:dyDescent="0.45">
+    <row r="19" spans="2:11" x14ac:dyDescent="0.4">
       <c r="B19" s="1" t="s">
         <v>60</v>
       </c>
@@ -2172,7 +2195,7 @@
       </c>
       <c r="K19" s="1"/>
     </row>
-    <row r="20" spans="2:11" ht="102" x14ac:dyDescent="0.45">
+    <row r="20" spans="2:11" ht="104.4" x14ac:dyDescent="0.4">
       <c r="B20" s="1" t="s">
         <v>61</v>
       </c>
@@ -2202,7 +2225,7 @@
       </c>
       <c r="K20" s="1"/>
     </row>
-    <row r="21" spans="2:11" ht="102" x14ac:dyDescent="0.45">
+    <row r="21" spans="2:11" ht="104.4" x14ac:dyDescent="0.4">
       <c r="B21" s="1" t="s">
         <v>61</v>
       </c>
@@ -2232,7 +2255,7 @@
       </c>
       <c r="K21" s="1"/>
     </row>
-    <row r="22" spans="2:11" ht="102" x14ac:dyDescent="0.45">
+    <row r="22" spans="2:11" ht="104.4" x14ac:dyDescent="0.4">
       <c r="B22" s="1" t="s">
         <v>61</v>
       </c>
@@ -2262,7 +2285,7 @@
       </c>
       <c r="K22" s="1"/>
     </row>
-    <row r="23" spans="2:11" ht="34" x14ac:dyDescent="0.45">
+    <row r="23" spans="2:11" ht="34.799999999999997" x14ac:dyDescent="0.4">
       <c r="B23" s="1" t="s">
         <v>84</v>
       </c>
@@ -2290,7 +2313,7 @@
       </c>
       <c r="K23" s="1"/>
     </row>
-    <row r="24" spans="2:11" ht="34" x14ac:dyDescent="0.45">
+    <row r="24" spans="2:11" ht="34.799999999999997" x14ac:dyDescent="0.4">
       <c r="B24" s="1" t="s">
         <v>84</v>
       </c>
@@ -2318,7 +2341,7 @@
       </c>
       <c r="K24" s="1"/>
     </row>
-    <row r="25" spans="2:11" ht="51" x14ac:dyDescent="0.45">
+    <row r="25" spans="2:11" ht="52.2" x14ac:dyDescent="0.4">
       <c r="B25" s="1" t="s">
         <v>89</v>
       </c>
@@ -2346,7 +2369,7 @@
       </c>
       <c r="K25" s="1"/>
     </row>
-    <row r="26" spans="2:11" ht="51" x14ac:dyDescent="0.45">
+    <row r="26" spans="2:11" ht="52.2" x14ac:dyDescent="0.4">
       <c r="B26" s="1" t="s">
         <v>89</v>
       </c>
@@ -2374,7 +2397,7 @@
       </c>
       <c r="K26" s="1"/>
     </row>
-    <row r="27" spans="2:11" ht="34" x14ac:dyDescent="0.45">
+    <row r="27" spans="2:11" ht="34.799999999999997" x14ac:dyDescent="0.4">
       <c r="B27" s="1" t="s">
         <v>90</v>
       </c>
@@ -2402,7 +2425,7 @@
       </c>
       <c r="K27" s="1"/>
     </row>
-    <row r="28" spans="2:11" ht="51" x14ac:dyDescent="0.45">
+    <row r="28" spans="2:11" ht="34.799999999999997" x14ac:dyDescent="0.4">
       <c r="B28" s="1" t="s">
         <v>90</v>
       </c>
@@ -2430,7 +2453,7 @@
       </c>
       <c r="K28" s="1"/>
     </row>
-    <row r="29" spans="2:11" ht="75.5" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="29" spans="2:11" ht="75.45" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B29" s="1" t="s">
         <v>98</v>
       </c>
@@ -2460,7 +2483,7 @@
       </c>
       <c r="K29" s="1"/>
     </row>
-    <row r="30" spans="2:11" ht="34" x14ac:dyDescent="0.45">
+    <row r="30" spans="2:11" ht="34.799999999999997" x14ac:dyDescent="0.4">
       <c r="B30" s="1" t="s">
         <v>106</v>
       </c>
@@ -2490,7 +2513,7 @@
       </c>
       <c r="K30" s="1"/>
     </row>
-    <row r="31" spans="2:11" ht="34" x14ac:dyDescent="0.45">
+    <row r="31" spans="2:11" ht="34.799999999999997" x14ac:dyDescent="0.4">
       <c r="B31" s="1" t="s">
         <v>106</v>
       </c>
@@ -2520,7 +2543,7 @@
       </c>
       <c r="K31" s="1"/>
     </row>
-    <row r="32" spans="2:11" ht="34" x14ac:dyDescent="0.45">
+    <row r="32" spans="2:11" ht="34.799999999999997" x14ac:dyDescent="0.4">
       <c r="B32" s="1" t="s">
         <v>106</v>
       </c>
@@ -2550,7 +2573,7 @@
       </c>
       <c r="K32" s="1"/>
     </row>
-    <row r="33" spans="2:11" ht="51" x14ac:dyDescent="0.45">
+    <row r="33" spans="2:11" ht="52.2" x14ac:dyDescent="0.4">
       <c r="B33" s="1" t="s">
         <v>119</v>
       </c>
@@ -2580,7 +2603,7 @@
       </c>
       <c r="K33" s="1"/>
     </row>
-    <row r="34" spans="2:11" ht="51" x14ac:dyDescent="0.45">
+    <row r="34" spans="2:11" ht="52.2" x14ac:dyDescent="0.4">
       <c r="B34" s="1" t="s">
         <v>119</v>
       </c>
@@ -2610,7 +2633,7 @@
       </c>
       <c r="K34" s="1"/>
     </row>
-    <row r="35" spans="2:11" ht="34" x14ac:dyDescent="0.45">
+    <row r="35" spans="2:11" ht="34.799999999999997" x14ac:dyDescent="0.4">
       <c r="B35" s="1" t="s">
         <v>125</v>
       </c>
@@ -2640,7 +2663,7 @@
       </c>
       <c r="K35" s="1"/>
     </row>
-    <row r="36" spans="2:11" ht="51" x14ac:dyDescent="0.45">
+    <row r="36" spans="2:11" ht="34.799999999999997" x14ac:dyDescent="0.4">
       <c r="B36" s="1" t="s">
         <v>130</v>
       </c>
@@ -2670,7 +2693,7 @@
       </c>
       <c r="K36" s="1"/>
     </row>
-    <row r="37" spans="2:11" ht="51" x14ac:dyDescent="0.45">
+    <row r="37" spans="2:11" ht="34.799999999999997" x14ac:dyDescent="0.4">
       <c r="B37" s="1" t="s">
         <v>135</v>
       </c>
@@ -2700,7 +2723,7 @@
       </c>
       <c r="K37" s="1"/>
     </row>
-    <row r="38" spans="2:11" x14ac:dyDescent="0.45">
+    <row r="38" spans="2:11" x14ac:dyDescent="0.4">
       <c r="B38" s="1" t="s">
         <v>141</v>
       </c>
@@ -2728,7 +2751,7 @@
       </c>
       <c r="K38" s="1"/>
     </row>
-    <row r="39" spans="2:11" ht="102" x14ac:dyDescent="0.45">
+    <row r="39" spans="2:11" ht="104.4" x14ac:dyDescent="0.4">
       <c r="B39" s="1" t="s">
         <v>145</v>
       </c>
@@ -2758,7 +2781,7 @@
       </c>
       <c r="K39" s="1"/>
     </row>
-    <row r="40" spans="2:11" ht="102" x14ac:dyDescent="0.45">
+    <row r="40" spans="2:11" ht="104.4" x14ac:dyDescent="0.4">
       <c r="B40" s="1" t="s">
         <v>145</v>
       </c>
@@ -2788,7 +2811,7 @@
       </c>
       <c r="K40" s="1"/>
     </row>
-    <row r="41" spans="2:11" ht="51" x14ac:dyDescent="0.45">
+    <row r="41" spans="2:11" ht="52.2" x14ac:dyDescent="0.4">
       <c r="B41" s="1" t="s">
         <v>146</v>
       </c>
@@ -2818,7 +2841,7 @@
       </c>
       <c r="K41" s="1"/>
     </row>
-    <row r="42" spans="2:11" x14ac:dyDescent="0.45">
+    <row r="42" spans="2:11" x14ac:dyDescent="0.4">
       <c r="J42"/>
     </row>
   </sheetData>

</xml_diff>